<commit_message>
updated existing generation for THI2 station
</commit_message>
<xml_diff>
--- a/lib/assets/202101_existing_generating_plant.xlsx
+++ b/lib/assets/202101_existing_generating_plant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevetorrens/workspace-ror/ghgemissions/lib/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D103C7-1793-AA49-A3DE-267798583EEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89BABFD-8F03-354C-A0CA-AAA0971867B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Connection Type Definitions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Generating Stations'!$A$1:$J$85</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Generating Stations'!$A$1:$E$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Generating Stations'!$A$1:$J$86</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Generating Stations'!$A$1:$E$84</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Generating Stations'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="219">
   <si>
     <t>Te Rere Hau</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>THI2201 THI1</t>
+  </si>
+  <si>
+    <t>THI2201 THI2</t>
   </si>
   <si>
     <t>WRK0331 TAA0</t>
@@ -1244,16 +1247,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1" filterMode="1">
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F26" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H38" sqref="H38"/>
+      <selection pane="bottomRight" activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1290,24 +1293,24 @@
         <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" hidden="1">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -1319,16 +1322,16 @@
         <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G2" s="27"/>
       <c r="H2" s="22"/>
       <c r="I2" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:10" hidden="1">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -1345,16 +1348,16 @@
         <v>196.7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="21"/>
       <c r="I3" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:10" hidden="1">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
@@ -1371,16 +1374,16 @@
         <v>196.7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="21"/>
       <c r="I4" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" hidden="1">
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
         <v>88</v>
       </c>
@@ -1397,16 +1400,16 @@
         <v>78</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="21"/>
       <c r="I5" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" hidden="1">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>89</v>
       </c>
@@ -1423,16 +1426,16 @@
         <v>3.8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="21"/>
       <c r="I6" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" hidden="1">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -1449,16 +1452,16 @@
         <v>84</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="21"/>
       <c r="I7" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" hidden="1">
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
@@ -1475,16 +1478,16 @@
         <v>220</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="21"/>
       <c r="I8" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" hidden="1">
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -1501,16 +1504,16 @@
         <v>540</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="21"/>
       <c r="I9" s="10" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" hidden="1">
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>94</v>
       </c>
@@ -1527,7 +1530,7 @@
         <v>432</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="21"/>
@@ -1536,7 +1539,7 @@
       </c>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" hidden="1">
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>96</v>
       </c>
@@ -1553,16 +1556,16 @@
         <v>32</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="21"/>
       <c r="I11" s="10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" hidden="1">
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>97</v>
       </c>
@@ -1579,16 +1582,16 @@
         <v>45</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="21"/>
       <c r="I12" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" hidden="1">
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
         <v>98</v>
       </c>
@@ -1605,16 +1608,16 @@
         <v>3.5</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="21"/>
       <c r="I13" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" hidden="1">
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>99</v>
       </c>
@@ -1631,16 +1634,16 @@
         <v>0.5</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="21"/>
       <c r="I14" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" hidden="1">
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
         <v>100</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>112</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G15" s="2">
         <v>0</v>
@@ -1668,7 +1671,7 @@
       </c>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" hidden="1">
+    <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
@@ -1685,16 +1688,16 @@
         <v>25.2</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="21"/>
       <c r="I16" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" hidden="1">
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -1711,7 +1714,7 @@
         <v>240</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G17" s="2">
         <v>10900</v>
@@ -1721,10 +1724,10 @@
         <v>110</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" hidden="1">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -1741,20 +1744,20 @@
         <v>240</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G18" s="2">
         <v>10900</v>
       </c>
       <c r="H18" s="21"/>
       <c r="I18" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" hidden="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>240</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G19" s="2">
         <v>10900</v>
@@ -1781,10 +1784,10 @@
         <v>111</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" hidden="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>4</v>
       </c>
@@ -1801,7 +1804,7 @@
         <v>400</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G20" s="2">
         <v>7400</v>
@@ -1811,10 +1814,10 @@
         <v>112</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>48</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G21" s="2">
         <v>10525</v>
@@ -1841,12 +1844,12 @@
         <v>123</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" hidden="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>29</v>
@@ -1861,16 +1864,16 @@
         <v>38</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="21"/>
       <c r="I22" s="10" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="1:10" hidden="1">
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
@@ -1887,16 +1890,16 @@
         <v>36</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="21"/>
       <c r="I23" s="10" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J23" s="10"/>
     </row>
-    <row r="24" spans="1:10" hidden="1">
+    <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>25</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G24" s="19">
         <f>10365*1.05506</f>
@@ -1924,10 +1927,10 @@
         <v>125</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -1944,12 +1947,12 @@
         <v>90</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="21"/>
       <c r="I25" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J25" s="10"/>
     </row>
@@ -1970,7 +1973,7 @@
         <v>37</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="21">
@@ -1984,7 +1987,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>36</v>
@@ -1999,7 +2002,7 @@
         <v>100</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="21">
@@ -2010,10 +2013,10 @@
         <v>114</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" hidden="1">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
@@ -2030,16 +2033,16 @@
         <v>28</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="21"/>
       <c r="I28" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="1:10" hidden="1">
+    <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -2056,7 +2059,7 @@
         <v>69.599999999999994</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G29" s="2">
         <v>9300</v>
@@ -2066,10 +2069,10 @@
         <v>113</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" hidden="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
         <v>44</v>
       </c>
@@ -2086,16 +2089,16 @@
         <v>6.5</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="21"/>
       <c r="I30" s="10" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J30" s="10"/>
     </row>
-    <row r="31" spans="1:10" hidden="1">
+    <row r="31" spans="1:10">
       <c r="A31" s="3" t="s">
         <v>17</v>
       </c>
@@ -2112,16 +2115,16 @@
         <v>36</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="21"/>
       <c r="I31" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J31" s="10"/>
     </row>
-    <row r="32" spans="1:10" hidden="1">
+    <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -2138,16 +2141,16 @@
         <v>850</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="21"/>
       <c r="I32" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:10" hidden="1">
+    <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
@@ -2164,16 +2167,16 @@
         <v>42</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="21"/>
       <c r="I33" s="10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:10" hidden="1">
+    <row r="34" spans="1:10">
       <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
@@ -2190,16 +2193,16 @@
         <v>360</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="21"/>
       <c r="I34" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:10" hidden="1">
+    <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
         <v>50</v>
       </c>
@@ -2216,16 +2219,16 @@
         <v>72</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="21"/>
       <c r="I35" s="10" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J35" s="10"/>
     </row>
-    <row r="36" spans="1:10" hidden="1">
+    <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
         <v>106</v>
       </c>
@@ -2242,7 +2245,7 @@
         <v>102</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G36" s="2">
         <f>G57</f>
@@ -2253,10 +2256,10 @@
         <v>126</v>
       </c>
       <c r="J36" s="25" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="3" t="s">
         <v>108</v>
       </c>
@@ -2273,12 +2276,12 @@
         <v>71.3</v>
       </c>
       <c r="F37" s="28" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="21"/>
       <c r="I37" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J37" s="10"/>
     </row>
@@ -2287,7 +2290,7 @@
         <v>48</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>37</v>
@@ -2299,7 +2302,7 @@
         <v>112</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="21">
@@ -2310,7 +2313,7 @@
         <v>121</v>
       </c>
       <c r="J38" s="25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2318,7 +2321,7 @@
         <v>16</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>37</v>
@@ -2330,7 +2333,7 @@
         <v>140</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="21">
@@ -2341,7 +2344,7 @@
         <v>115</v>
       </c>
       <c r="J39" s="25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2361,7 +2364,7 @@
         <v>82</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="21">
@@ -2372,7 +2375,7 @@
         <v>127</v>
       </c>
       <c r="J40" s="25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2392,7 +2395,7 @@
         <v>25</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="26">
@@ -2400,10 +2403,10 @@
         <v>0.307</v>
       </c>
       <c r="I41" s="20" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J41" s="25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2423,7 +2426,7 @@
         <v>70</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="21">
@@ -2434,10 +2437,10 @@
         <v>116</v>
       </c>
       <c r="J42" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" hidden="1">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
         <v>54</v>
       </c>
@@ -2454,16 +2457,16 @@
         <v>112</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="21"/>
       <c r="I43" s="10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="1:10" hidden="1">
+    <row r="44" spans="1:10">
       <c r="A44" s="2" t="s">
         <v>55</v>
       </c>
@@ -2480,16 +2483,16 @@
         <v>264</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="21"/>
       <c r="I44" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J44" s="10"/>
     </row>
-    <row r="45" spans="1:10" hidden="1">
+    <row r="45" spans="1:10">
       <c r="A45" s="2" t="s">
         <v>56</v>
       </c>
@@ -2506,16 +2509,16 @@
         <v>212</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="21"/>
       <c r="I45" s="10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J45" s="10"/>
     </row>
-    <row r="46" spans="1:10" hidden="1">
+    <row r="46" spans="1:10">
       <c r="A46" s="2" t="s">
         <v>57</v>
       </c>
@@ -2532,16 +2535,16 @@
         <v>212</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="21"/>
       <c r="I46" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J46" s="10"/>
     </row>
-    <row r="47" spans="1:10" hidden="1">
+    <row r="47" spans="1:10">
       <c r="A47" s="2" t="s">
         <v>58</v>
       </c>
@@ -2558,16 +2561,16 @@
         <v>30.7</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="21"/>
       <c r="I47" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J47" s="10"/>
     </row>
-    <row r="48" spans="1:10" hidden="1">
+    <row r="48" spans="1:10">
       <c r="A48" s="2" t="s">
         <v>58</v>
       </c>
@@ -2584,16 +2587,16 @@
         <v>30.7</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="21"/>
       <c r="I48" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J48" s="10"/>
     </row>
-    <row r="49" spans="1:10" hidden="1">
+    <row r="49" spans="1:10">
       <c r="A49" s="2" t="s">
         <v>58</v>
       </c>
@@ -2610,16 +2613,16 @@
         <v>30.7</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="21"/>
       <c r="I49" s="10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J49" s="10"/>
     </row>
-    <row r="50" spans="1:10" hidden="1">
+    <row r="50" spans="1:10">
       <c r="A50" s="2" t="s">
         <v>59</v>
       </c>
@@ -2636,16 +2639,16 @@
         <v>2.25</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="21"/>
       <c r="I50" s="10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J50" s="10"/>
     </row>
-    <row r="51" spans="1:10" hidden="1">
+    <row r="51" spans="1:10">
       <c r="A51" s="2" t="s">
         <v>60</v>
       </c>
@@ -2662,12 +2665,12 @@
         <v>42</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="21"/>
       <c r="I51" s="10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J51" s="10"/>
     </row>
@@ -2688,7 +2691,7 @@
         <v>55</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="21">
@@ -2699,10 +2702,10 @@
         <v>117</v>
       </c>
       <c r="J52" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" hidden="1">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="2" t="s">
         <v>62</v>
       </c>
@@ -2719,12 +2722,12 @@
         <v>120</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="21"/>
       <c r="I53" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J53" s="10"/>
     </row>
@@ -2745,7 +2748,7 @@
         <v>33</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="21">
@@ -2753,13 +2756,13 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J54" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" hidden="1">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="2" t="s">
         <v>64</v>
       </c>
@@ -2776,7 +2779,7 @@
         <v>320</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="21"/>
@@ -2785,7 +2788,7 @@
       </c>
       <c r="J55" s="10"/>
     </row>
-    <row r="56" spans="1:10" hidden="1">
+    <row r="56" spans="1:10">
       <c r="A56" s="2" t="s">
         <v>64</v>
       </c>
@@ -2802,7 +2805,7 @@
         <v>320</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="21"/>
@@ -2811,7 +2814,7 @@
       </c>
       <c r="J56" s="10"/>
     </row>
-    <row r="57" spans="1:10" hidden="1">
+    <row r="57" spans="1:10">
       <c r="A57" s="3" t="s">
         <v>105</v>
       </c>
@@ -2828,7 +2831,7 @@
         <v>100</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G57" s="2">
         <v>8907</v>
@@ -2838,15 +2841,15 @@
         <v>124</v>
       </c>
       <c r="J57" s="25" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" hidden="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>27</v>
@@ -2858,21 +2861,21 @@
         <v>31.7</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="21"/>
       <c r="I58" s="10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J58" s="10"/>
     </row>
-    <row r="59" spans="1:10" hidden="1">
+    <row r="59" spans="1:10">
       <c r="A59" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>27</v>
@@ -2884,21 +2887,21 @@
         <v>36.299999999999997</v>
       </c>
       <c r="F59" s="28" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="21"/>
       <c r="I59" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J59" s="10"/>
     </row>
-    <row r="60" spans="1:10" hidden="1">
+    <row r="60" spans="1:10">
       <c r="A60" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>37</v>
@@ -2910,16 +2913,16 @@
         <v>93</v>
       </c>
       <c r="F60" s="28" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="21"/>
       <c r="I60" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J60" s="10"/>
     </row>
-    <row r="61" spans="1:10" hidden="1">
+    <row r="61" spans="1:10">
       <c r="A61" s="3" t="s">
         <v>105</v>
       </c>
@@ -2936,7 +2939,7 @@
         <v>100</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G61" s="2">
         <f>G57</f>
@@ -2947,10 +2950,10 @@
         <v>118</v>
       </c>
       <c r="J61" s="25" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" hidden="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="2" t="s">
         <v>68</v>
       </c>
@@ -2967,7 +2970,7 @@
         <v>385</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G62" s="2">
         <v>7400</v>
@@ -2977,10 +2980,10 @@
         <v>119</v>
       </c>
       <c r="J62" s="25" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" hidden="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="2" t="s">
         <v>69</v>
       </c>
@@ -2997,12 +3000,12 @@
         <v>90.75</v>
       </c>
       <c r="F63" s="28" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="21"/>
       <c r="I63" s="10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J63" s="10"/>
     </row>
@@ -3023,7 +3026,7 @@
         <v>23</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="21">
@@ -3031,10 +3034,10 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J64" s="25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -3054,7 +3057,7 @@
         <v>166</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="21">
@@ -3065,120 +3068,125 @@
         <v>132</v>
       </c>
       <c r="J65" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" hidden="1">
-      <c r="A66" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="2">
+        <v>166</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="21">
+        <f>H65</f>
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="J66" s="25" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E66" s="2">
-        <v>44</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="G66" s="2">
-        <v>11700</v>
-      </c>
-      <c r="H66" s="21"/>
-      <c r="I66" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="J66" s="25" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" hidden="1">
-      <c r="A67" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="E67" s="2">
-        <v>48.5</v>
-      </c>
-      <c r="F67" s="28" t="s">
-        <v>217</v>
-      </c>
-      <c r="G67" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G67" s="2">
+        <v>11700</v>
+      </c>
       <c r="H67" s="21"/>
       <c r="I67" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="J67" s="10"/>
-    </row>
-    <row r="68" spans="1:10" hidden="1">
-      <c r="A68" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D68" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J67" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>93</v>
       </c>
       <c r="E68" s="2">
-        <v>64.400000000000006</v>
+        <v>48.5</v>
       </c>
       <c r="F68" s="28" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G68" s="2"/>
       <c r="H68" s="21"/>
       <c r="I68" s="10" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="J68" s="10"/>
     </row>
-    <row r="69" spans="1:10" hidden="1">
-      <c r="A69" s="2" t="s">
-        <v>80</v>
+    <row r="69" spans="1:10">
+      <c r="A69" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E69" s="2">
-        <v>25</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>214</v>
+        <v>64.400000000000006</v>
+      </c>
+      <c r="F69" s="28" t="s">
+        <v>218</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="21"/>
       <c r="I69" s="10" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="J69" s="10"/>
     </row>
-    <row r="70" spans="1:10" hidden="1">
+    <row r="70" spans="1:10">
       <c r="A70" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>102</v>
@@ -3190,10 +3198,10 @@
         <v>34</v>
       </c>
       <c r="E70" s="2">
-        <v>160</v>
+        <v>25</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="21"/>
@@ -3202,11 +3210,11 @@
       </c>
       <c r="J70" s="10"/>
     </row>
-    <row r="71" spans="1:10" hidden="1">
+    <row r="71" spans="1:10">
       <c r="A71" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B71" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -3216,10 +3224,10 @@
         <v>34</v>
       </c>
       <c r="E71" s="2">
-        <v>240</v>
+        <v>160</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="21"/>
@@ -3228,9 +3236,9 @@
       </c>
       <c r="J71" s="10"/>
     </row>
-    <row r="72" spans="1:10" hidden="1">
+    <row r="72" spans="1:10">
       <c r="A72" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>102</v>
@@ -3242,24 +3250,24 @@
         <v>34</v>
       </c>
       <c r="E72" s="2">
-        <v>60</v>
+        <v>240</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G72" s="2"/>
       <c r="H72" s="21"/>
       <c r="I72" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J72" s="10"/>
     </row>
-    <row r="73" spans="1:10" hidden="1">
+    <row r="73" spans="1:10">
       <c r="A73" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>37</v>
@@ -3268,145 +3276,145 @@
         <v>34</v>
       </c>
       <c r="E73" s="2">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="21"/>
       <c r="I73" s="10" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="J73" s="10"/>
     </row>
-    <row r="74" spans="1:10" hidden="1">
+    <row r="74" spans="1:10">
       <c r="A74" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E74" s="2">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="21"/>
       <c r="I74" s="10" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="J74" s="10"/>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" s="2">
+        <v>84</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G75" s="2"/>
+      <c r="H75" s="21"/>
+      <c r="I75" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="J75" s="10"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D75" s="28" t="s">
+      <c r="C76" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D76" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E76" s="2">
         <v>161</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G75" s="2"/>
-      <c r="H75" s="21">
+      <c r="F76" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G76" s="2"/>
+      <c r="H76" s="21">
         <f>21/1000</f>
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="I75" s="10" t="s">
+      <c r="I76" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="J75" s="25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" hidden="1">
-      <c r="A76" s="2" t="s">
+      <c r="J76" s="25" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E76" s="2">
+      <c r="D77" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="2">
         <v>84</v>
       </c>
-      <c r="F76" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="G76" s="2"/>
-      <c r="H76" s="21"/>
-      <c r="I76" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="J76" s="10"/>
-    </row>
-    <row r="77" spans="1:10" hidden="1">
-      <c r="A77" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E77" s="2">
-        <v>90</v>
-      </c>
       <c r="F77" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="21"/>
       <c r="I77" s="10" t="s">
-        <v>148</v>
+        <v>187</v>
       </c>
       <c r="J77" s="10"/>
     </row>
-    <row r="78" spans="1:10" hidden="1">
-      <c r="A78" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B78" s="3" t="s">
+    <row r="78" spans="1:10">
+      <c r="A78" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D78" s="3" t="s">
-        <v>93</v>
+      <c r="D78" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E78" s="2">
-        <v>143</v>
-      </c>
-      <c r="F78" s="28" t="s">
-        <v>217</v>
+        <v>90</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="21"/>
@@ -3415,205 +3423,225 @@
       </c>
       <c r="J78" s="10"/>
     </row>
-    <row r="79" spans="1:10" hidden="1">
-      <c r="A79" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>36</v>
+    <row r="79" spans="1:10">
+      <c r="A79" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>34</v>
+      <c r="D79" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E79" s="2">
-        <v>100</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>214</v>
+        <v>143</v>
+      </c>
+      <c r="F79" s="28" t="s">
+        <v>218</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="21"/>
       <c r="I79" s="10" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="J79" s="10"/>
     </row>
-    <row r="80" spans="1:10" hidden="1">
-      <c r="A80" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>26</v>
+    <row r="80" spans="1:10">
+      <c r="A80" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>93</v>
+      <c r="D80" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E80" s="2">
-        <v>143</v>
-      </c>
-      <c r="F80" s="28" t="s">
-        <v>217</v>
+        <v>100</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="21"/>
       <c r="I80" s="10" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="J80" s="10"/>
     </row>
-    <row r="81" spans="1:10" hidden="1">
-      <c r="A81" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>29</v>
+    <row r="81" spans="1:10">
+      <c r="A81" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>34</v>
+      <c r="D81" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E81" s="2">
-        <v>24</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>214</v>
+        <v>143</v>
+      </c>
+      <c r="F81" s="28" t="s">
+        <v>218</v>
       </c>
       <c r="G81" s="2"/>
       <c r="H81" s="21"/>
       <c r="I81" s="10" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="J81" s="10"/>
     </row>
-    <row r="82" spans="1:10" hidden="1">
+    <row r="82" spans="1:10">
       <c r="A82" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E82" s="2">
-        <v>155</v>
-      </c>
-      <c r="F82" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="G82" s="2">
-        <v>10906</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G82" s="2"/>
       <c r="H82" s="21"/>
       <c r="I82" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="J82" s="25" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" hidden="1">
+        <v>172</v>
+      </c>
+      <c r="J82" s="10"/>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="E83" s="2">
-        <v>58</v>
-      </c>
-      <c r="F83" s="28" t="s">
-        <v>217</v>
-      </c>
-      <c r="G83" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="F83" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="G83" s="2">
+        <v>10906</v>
+      </c>
       <c r="H83" s="21"/>
       <c r="I83" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="J83" s="10"/>
-    </row>
-    <row r="84" spans="1:10" hidden="1">
-      <c r="A84" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="C84" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D84" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="J83" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E84" s="11">
+      <c r="E84" s="2">
+        <v>58</v>
+      </c>
+      <c r="F84" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="G84" s="2"/>
+      <c r="H84" s="21"/>
+      <c r="I84" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="J84" s="10"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D85" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E85" s="11">
         <v>133</v>
       </c>
-      <c r="F84" s="28" t="s">
-        <v>217</v>
-      </c>
-      <c r="G84" s="23"/>
-      <c r="H84" s="23"/>
-      <c r="I84" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="J84" s="10"/>
-    </row>
-    <row r="85" spans="1:10" hidden="1">
-      <c r="A85" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="B85" s="13" t="s">
+      <c r="F85" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="G85" s="23"/>
+      <c r="H85" s="23"/>
+      <c r="I85" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="J85" s="10"/>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B86" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C85" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D85" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E85" s="17">
+      <c r="C86" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="E86" s="17">
         <v>100</v>
       </c>
-      <c r="F85" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="G85" s="23">
+      <c r="F86" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="G86" s="23">
         <f>G57</f>
         <v>8907</v>
       </c>
-      <c r="H85" s="23"/>
-      <c r="I85" s="25" t="s">
-        <v>202</v>
-      </c>
-      <c r="J85" s="25" t="s">
-        <v>196</v>
+      <c r="H86" s="23"/>
+      <c r="I86" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="J86" s="25" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J85" xr:uid="{9418BDBF-9512-7747-866E-C1A7EBFD53C1}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="geothermal"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J86" xr:uid="{9418BDBF-9512-7747-866E-C1A7EBFD53C1}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.17" right="0.22" top="0.66" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="8" scale="74" fitToHeight="0" orientation="portrait"/>

</xml_diff>

<commit_message>
updated generation spreadsheet Southdown
</commit_message>
<xml_diff>
--- a/lib/assets/202101_existing_generating_plant.xlsx
+++ b/lib/assets/202101_existing_generating_plant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevetorrens/workspace-ror/ghgemissions/lib/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89BABFD-8F03-354C-A0CA-AAA0971867B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466CDB1A-3955-7343-871E-C496E7749ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generating Stations" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="222">
   <si>
     <t>Te Rere Hau</t>
   </si>
@@ -694,6 +694,15 @@
   </si>
   <si>
     <t>wind</t>
+  </si>
+  <si>
+    <t>SWN2201 SWN1</t>
+  </si>
+  <si>
+    <t>Southdown Battery</t>
+  </si>
+  <si>
+    <t>Battery</t>
   </si>
 </sst>
 </file>
@@ -870,7 +879,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
@@ -908,6 +917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1250,13 +1260,13 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E66" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A65" sqref="A65"/>
+      <selection pane="bottomRight" activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3619,8 +3629,8 @@
       <c r="C86" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D86" s="15" t="s">
-        <v>208</v>
+      <c r="D86" s="29" t="s">
+        <v>30</v>
       </c>
       <c r="E86" s="17">
         <v>100</v>
@@ -3638,6 +3648,29 @@
       </c>
       <c r="J86" s="25" t="s">
         <v>197</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E87" s="17">
+        <v>1</v>
+      </c>
+      <c r="F87" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="I87" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>